<commit_message>
Feedback Map and Project Status Updated
</commit_message>
<xml_diff>
--- a/Feedback Map.xlsx
+++ b/Feedback Map.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE0EEDA6-ACC6-43A9-9CA6-3439CABDFA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17863A84-3A88-4E9E-A88F-50A963DDCE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Self</t>
+  </si>
+  <si>
+    <t>Stand Up recording, as advised by Module 3.4 is not required for PortfolioRecord this stand-up and add it to your portfolio</t>
+  </si>
+  <si>
+    <t>Removed the stand Up Recording from Portfolio</t>
   </si>
 </sst>
 </file>
@@ -504,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -640,33 +646,45 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" s="10" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
-        <v>44984</v>
+        <v>44977</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
+        <v>44984</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F8" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
@@ -748,8 +766,24 @@
       <c r="E18" s="6"/>
       <c r="F18" s="5"/>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="5"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:XFD2 A3:F18">
+  <conditionalFormatting sqref="A2:XFD2 A3:F20">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>$F2="Completed"</formula>
     </cfRule>
@@ -761,7 +795,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F18" xr:uid="{A60926BB-C77F-420F-BD81-A06577EBA7E4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F20" xr:uid="{A60926BB-C77F-420F-BD81-A06577EBA7E4}">
       <formula1>"Not Started, In Progress, Completed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -921,18 +955,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -954,18 +988,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBB0FCED-7504-4C40-A973-53ACEBC7B3CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742EE796-58C4-4EC2-BE72-8477364E6924}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBB0FCED-7504-4C40-A973-53ACEBC7B3CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>